<commit_message>
Prepare for importing formula expressions to the model.
</commit_message>
<xml_diff>
--- a/test/xlsx/test.xlsx
+++ b/test/xlsx/test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Simple Format" sheetId="2" r:id="rId2"/>
     <sheet name="Formula" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1115,6 +1115,13 @@
       </c>
     </row>
     <row r="5" spans="1:7">
+      <c r="A5" t="str">
+        <f>CONCATENATE("MW","-",B5)</f>
+        <v>MW-10</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
       <c r="D5">
         <v>5</v>
       </c>
@@ -1128,6 +1135,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
+      <c r="A6" t="str">
+        <f t="shared" ref="A6:A13" si="2">CONCATENATE("MW","-",B6)</f>
+        <v>MW-11</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
       <c r="D6">
         <v>6</v>
       </c>
@@ -1141,6 +1155,13 @@
       </c>
     </row>
     <row r="7" spans="1:7">
+      <c r="A7" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-12</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
       <c r="D7">
         <v>7</v>
       </c>
@@ -1154,6 +1175,13 @@
       </c>
     </row>
     <row r="8" spans="1:7">
+      <c r="A8" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-13</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
       <c r="D8">
         <v>8</v>
       </c>
@@ -1167,6 +1195,13 @@
       </c>
     </row>
     <row r="9" spans="1:7">
+      <c r="A9" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-14</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
       <c r="D9">
         <v>9</v>
       </c>
@@ -1180,6 +1215,13 @@
       </c>
     </row>
     <row r="10" spans="1:7">
+      <c r="A10" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-15</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
       <c r="D10">
         <v>10</v>
       </c>
@@ -1193,6 +1235,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
+      <c r="A11" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-16</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
       <c r="D11">
         <v>11</v>
       </c>
@@ -1206,6 +1255,13 @@
       </c>
     </row>
     <row r="12" spans="1:7">
+      <c r="A12" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-17</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
       <c r="D12">
         <v>12</v>
       </c>
@@ -1219,6 +1275,13 @@
       </c>
     </row>
     <row r="13" spans="1:7">
+      <c r="A13" t="str">
+        <f t="shared" si="2"/>
+        <v>MW-18</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
       <c r="D13">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Keep it consistent in configure.ac & test files updated.
</commit_message>
<xml_diff>
--- a/test/xlsx/test.xlsx
+++ b/test/xlsx/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815"/>
   </bookViews>
   <sheets>
     <sheet name="Unformatted" sheetId="1" r:id="rId1"/>
@@ -812,11 +812,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="4" max="10" width="6.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -903,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="40.5" customHeight="1">
       <c r="D10">
         <v>11.1</v>
       </c>
@@ -913,7 +917,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="24" customHeight="1">
       <c r="F12">
         <v>33.299999999999997</v>
       </c>
@@ -1044,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Import merged cell ranges from xlsx.
</commit_message>
<xml_diff>
--- a/test/xlsx/test.xlsx
+++ b/test/xlsx/test.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="16080" windowHeight="10815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Unformatted" sheetId="1" r:id="rId1"/>
     <sheet name="Simple Format" sheetId="2" r:id="rId2"/>
     <sheet name="Formula" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -315,6 +315,21 @@
   </si>
   <si>
     <t>Background colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>light green</t>
   </si>
 </sst>
 </file>
@@ -499,12 +514,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -516,6 +529,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -946,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,19 +1004,27 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="92.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="46.5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="92.25">
-      <c r="A6" t="s">
+      <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="35.25">
       <c r="A7" t="s">
@@ -1007,22 +1037,22 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1032,13 +1062,28 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Skip cells that are overlapped by merged cells in html output.
</commit_message>
<xml_diff>
--- a/test/xlsx/test.xlsx
+++ b/test/xlsx/test.xlsx
@@ -214,6 +214,45 @@
     </r>
   </si>
   <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>outline</t>
+  </si>
+  <si>
+    <t>Borders</t>
+  </si>
+  <si>
+    <t>Background colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>light green</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Calibri </t>
     </r>
@@ -289,47 +328,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>oman</t>
-    </r>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>outline</t>
-  </si>
-  <si>
-    <t>Borders</t>
-  </si>
-  <si>
-    <t>Background colors</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
-    <t>light green</t>
+      <t>oman - right-aligned.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,6 +537,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,7 +972,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1027,62 +1030,68 @@
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="35.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Import 'top', 'center', 'bottom' vertical alignment from xlsx.
And use it in html output.  We still need to handle other vertical
alignment types.
</commit_message>
<xml_diff>
--- a/test/xlsx/test.xlsx
+++ b/test/xlsx/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -330,6 +330,15 @@
       </rPr>
       <t>oman - right-aligned.</t>
     </r>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Bottom</t>
   </si>
 </sst>
 </file>
@@ -413,7 +422,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,8 +459,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -510,11 +525,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,12 +582,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -969,19 +1025,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -992,7 +1049,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1006,21 +1063,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="92.25">
+    <row r="4" spans="1:8" ht="92.25">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" ht="46.5">
+      <c r="F4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="46.5">
       <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="92.25">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" ht="92.25">
       <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1098,7 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="35.25">
+    <row r="7" spans="1:8" ht="35.25">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
@@ -1039,12 +1108,12 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1064,12 +1133,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
@@ -1087,14 +1156,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>